<commit_message>
2018.8.27 0:53更新 Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/19秋招信息表.xlsx
+++ b/19秋招信息表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="公司列表" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="209">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -852,6 +852,10 @@
   </si>
   <si>
     <t>开始日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上海，软件开发工程师8个人</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1325,9 +1329,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2886,7 +2890,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3034,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3244,10 +3248,14 @@
       <c r="B17" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>

</xml_diff>